<commit_message>
Wat dingetjes toegevoegd en het wiskundig model wat meer python proof gemaakt
</commit_message>
<xml_diff>
--- a/paintshop_september_2024.xlsx
+++ b/paintshop_september_2024.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="33" documentId="11_907AF58AD413A54558041772E588C1D2BB2CC3E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6AEA5AA-67C7-4B7E-892B-8F7ADF2EF5DC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Orders!$A$1:$E$31</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentManualCount="20"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -463,7 +463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -1062,8 +1062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1222,15 +1222,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010013B620F01982514694878B55267266B0" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="b766b0002d27b841048f4e26ce56a6ad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="882bdec5-c3ce-4705-9a84-58ed8ad203ea" xmlns:ns3="c6fe3531-949f-4c96-ac1d-b793c48e3f25" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="19b1c955cd3d6da461c7724026070e4b" ns2:_="" ns3:_="">
     <xsd:import namespace="882bdec5-c3ce-4705-9a84-58ed8ad203ea"/>
@@ -1445,15 +1436,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2F853DD-D83E-469C-9E1E-915877D838F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AA6E6B3-C3FA-4A0D-B5D1-063D13496ACE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1470,4 +1462,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2F853DD-D83E-469C-9E1E-915877D838F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Constructive heuristics aan de praat gekregen. discrete improving search still a work in progress.
</commit_message>
<xml_diff>
--- a/paintshop_september_2024.xlsx
+++ b/paintshop_september_2024.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="33" documentId="11_907AF58AD413A54558041772E588C1D2BB2CC3E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6AEA5AA-67C7-4B7E-892B-8F7ADF2EF5DC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Orders!$A$1:$E$31</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentManualCount="20"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -463,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E1" sqref="A1:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1011,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1062,7 +1062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1222,6 +1222,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010013B620F01982514694878B55267266B0" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="b766b0002d27b841048f4e26ce56a6ad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="882bdec5-c3ce-4705-9a84-58ed8ad203ea" xmlns:ns3="c6fe3531-949f-4c96-ac1d-b793c48e3f25" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="19b1c955cd3d6da461c7724026070e4b" ns2:_="" ns3:_="">
     <xsd:import namespace="882bdec5-c3ce-4705-9a84-58ed8ad203ea"/>
@@ -1436,16 +1445,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2F853DD-D83E-469C-9E1E-915877D838F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AA6E6B3-C3FA-4A0D-B5D1-063D13496ACE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1462,12 +1470,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2F853DD-D83E-469C-9E1E-915877D838F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Constructive heurisitcs doet het nu echt
</commit_message>
<xml_diff>
--- a/paintshop_september_2024.xlsx
+++ b/paintshop_september_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/46d9bc8e4b2e6b05/Bureaublad/Fontys/DS5/VS code spul/OR5_/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="11_907AF58AD413A54558041772E588C1D2BB2CC3E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6AEA5AA-67C7-4B7E-892B-8F7ADF2EF5DC}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="11_907AF58AD413A54558041772E588C1D2BB2CC3E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F311DC17-821E-47BF-BE3E-1AC6F11702D6}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -463,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E1" sqref="A1:E31"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1011,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1222,15 +1222,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010013B620F01982514694878B55267266B0" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="b766b0002d27b841048f4e26ce56a6ad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="882bdec5-c3ce-4705-9a84-58ed8ad203ea" xmlns:ns3="c6fe3531-949f-4c96-ac1d-b793c48e3f25" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="19b1c955cd3d6da461c7724026070e4b" ns2:_="" ns3:_="">
     <xsd:import namespace="882bdec5-c3ce-4705-9a84-58ed8ad203ea"/>
@@ -1445,15 +1436,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2F853DD-D83E-469C-9E1E-915877D838F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AA6E6B3-C3FA-4A0D-B5D1-063D13496ACE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1470,4 +1462,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2F853DD-D83E-469C-9E1E-915877D838F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>